<commit_message>
Se realizó la creación de funciones para filtrar equipos por diferentes parametros y generar 10 tickets por zona
</commit_message>
<xml_diff>
--- a/data/lista_lima.xlsx
+++ b/data/lista_lima.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\snayd\Desktop\Dalia\gestion\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D59575F3-ED9D-4EDC-AB1C-DC0170C81D09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{555DC6B8-4ED9-49BA-A2B8-EA9FB82EE769}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1264" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1264" uniqueCount="279">
   <si>
     <t>PRIORIDAD</t>
   </si>
@@ -146,9 +146,6 @@
   </si>
   <si>
     <t>Alta</t>
-  </si>
-  <si>
-    <t>LI05769</t>
   </si>
   <si>
     <t>SAN_CRISTOBAL</t>
@@ -1318,7 +1315,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1673,10 +1670,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" t="s">
         <v>41</v>
-      </c>
-      <c r="C6" t="s">
-        <v>42</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>23</v>
@@ -1697,7 +1694,7 @@
         <v>24</v>
       </c>
       <c r="J6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K6" s="13">
         <v>-12.069165999999999</v>
@@ -1738,10 +1735,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" t="s">
         <v>44</v>
-      </c>
-      <c r="C7" t="s">
-        <v>45</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>23</v>
@@ -1762,7 +1759,7 @@
         <v>24</v>
       </c>
       <c r="J7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K7" s="13">
         <v>-11.995798000000001</v>
@@ -1803,10 +1800,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" t="s">
         <v>47</v>
-      </c>
-      <c r="C8" t="s">
-        <v>48</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>23</v>
@@ -1827,7 +1824,7 @@
         <v>24</v>
       </c>
       <c r="J8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K8" s="13">
         <v>-12.162544</v>
@@ -1868,10 +1865,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" t="s">
         <v>50</v>
-      </c>
-      <c r="C9" t="s">
-        <v>51</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>23</v>
@@ -1892,7 +1889,7 @@
         <v>24</v>
       </c>
       <c r="J9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K9" s="13">
         <v>-12.13191</v>
@@ -1933,10 +1930,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" t="s">
         <v>52</v>
-      </c>
-      <c r="C10" t="s">
-        <v>53</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>23</v>
@@ -1957,7 +1954,7 @@
         <v>24</v>
       </c>
       <c r="J10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K10" s="13">
         <v>-12.15652</v>
@@ -1998,10 +1995,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" t="s">
         <v>54</v>
-      </c>
-      <c r="C11" t="s">
-        <v>55</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>23</v>
@@ -2022,7 +2019,7 @@
         <v>24</v>
       </c>
       <c r="J11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K11" s="13">
         <v>-12.128600929999999</v>
@@ -2063,10 +2060,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" t="s">
         <v>56</v>
-      </c>
-      <c r="C12" t="s">
-        <v>57</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>23</v>
@@ -2128,10 +2125,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13" t="s">
         <v>58</v>
-      </c>
-      <c r="C13" t="s">
-        <v>59</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>23</v>
@@ -2193,10 +2190,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" t="s">
         <v>60</v>
-      </c>
-      <c r="C14" t="s">
-        <v>61</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>23</v>
@@ -2217,7 +2214,7 @@
         <v>24</v>
       </c>
       <c r="J14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K14" s="13">
         <v>-12.08919</v>
@@ -2241,7 +2238,7 @@
         <v>34</v>
       </c>
       <c r="R14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="S14" t="s">
         <v>28</v>
@@ -2258,10 +2255,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" t="s">
         <v>64</v>
-      </c>
-      <c r="C15" t="s">
-        <v>65</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>23</v>
@@ -2323,10 +2320,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
+        <v>65</v>
+      </c>
+      <c r="C16" t="s">
         <v>66</v>
-      </c>
-      <c r="C16" t="s">
-        <v>67</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>23</v>
@@ -2388,10 +2385,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
+        <v>67</v>
+      </c>
+      <c r="C17" t="s">
         <v>68</v>
-      </c>
-      <c r="C17" t="s">
-        <v>69</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>23</v>
@@ -2453,10 +2450,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
+        <v>69</v>
+      </c>
+      <c r="C18" t="s">
         <v>70</v>
-      </c>
-      <c r="C18" t="s">
-        <v>71</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>23</v>
@@ -2477,7 +2474,7 @@
         <v>24</v>
       </c>
       <c r="J18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K18" s="13">
         <v>-12.131688</v>
@@ -2518,10 +2515,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
+        <v>72</v>
+      </c>
+      <c r="C19" t="s">
         <v>73</v>
-      </c>
-      <c r="C19" t="s">
-        <v>74</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>23</v>
@@ -2539,10 +2536,10 @@
         <v>24</v>
       </c>
       <c r="I19" t="s">
+        <v>74</v>
+      </c>
+      <c r="J19" t="s">
         <v>75</v>
-      </c>
-      <c r="J19" t="s">
-        <v>76</v>
       </c>
       <c r="K19" s="13">
         <v>-12.061686</v>
@@ -2583,10 +2580,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
+        <v>76</v>
+      </c>
+      <c r="C20" t="s">
         <v>77</v>
-      </c>
-      <c r="C20" t="s">
-        <v>78</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>23</v>
@@ -2607,7 +2604,7 @@
         <v>24</v>
       </c>
       <c r="J20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K20" s="13">
         <v>-12.112333</v>
@@ -2648,10 +2645,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
+        <v>78</v>
+      </c>
+      <c r="C21" t="s">
         <v>79</v>
-      </c>
-      <c r="C21" t="s">
-        <v>80</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>23</v>
@@ -2713,10 +2710,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
+        <v>80</v>
+      </c>
+      <c r="C22" t="s">
         <v>81</v>
-      </c>
-      <c r="C22" t="s">
-        <v>82</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>23</v>
@@ -2761,7 +2758,7 @@
         <v>37</v>
       </c>
       <c r="R22" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="S22" t="s">
         <v>28</v>
@@ -2778,10 +2775,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
+        <v>82</v>
+      </c>
+      <c r="C23" t="s">
         <v>83</v>
-      </c>
-      <c r="C23" t="s">
-        <v>84</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>23</v>
@@ -2802,7 +2799,7 @@
         <v>24</v>
       </c>
       <c r="J23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K23" s="13">
         <v>-11.995279999999999</v>
@@ -2843,10 +2840,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
+        <v>84</v>
+      </c>
+      <c r="C24" t="s">
         <v>85</v>
-      </c>
-      <c r="C24" t="s">
-        <v>86</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>23</v>
@@ -2908,10 +2905,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
+        <v>86</v>
+      </c>
+      <c r="C25" t="s">
         <v>87</v>
-      </c>
-      <c r="C25" t="s">
-        <v>88</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>23</v>
@@ -2932,7 +2929,7 @@
         <v>24</v>
       </c>
       <c r="J25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K25" s="13">
         <v>-12.084425</v>
@@ -2973,10 +2970,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C26" t="s">
         <v>90</v>
-      </c>
-      <c r="C26" t="s">
-        <v>91</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>23</v>
@@ -2997,7 +2994,7 @@
         <v>24</v>
       </c>
       <c r="J26" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K26" s="13">
         <v>-12.08741</v>
@@ -3038,10 +3035,10 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
+        <v>91</v>
+      </c>
+      <c r="C27" t="s">
         <v>92</v>
-      </c>
-      <c r="C27" t="s">
-        <v>93</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>23</v>
@@ -3062,7 +3059,7 @@
         <v>24</v>
       </c>
       <c r="J27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K27" s="13">
         <v>-12.0814</v>
@@ -3103,10 +3100,10 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
+        <v>93</v>
+      </c>
+      <c r="C28" t="s">
         <v>94</v>
-      </c>
-      <c r="C28" t="s">
-        <v>95</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>23</v>
@@ -3127,7 +3124,7 @@
         <v>24</v>
       </c>
       <c r="J28" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K28" s="13">
         <v>-12.124651999999999</v>
@@ -3168,10 +3165,10 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
+        <v>95</v>
+      </c>
+      <c r="C29" t="s">
         <v>96</v>
-      </c>
-      <c r="C29" t="s">
-        <v>97</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>23</v>
@@ -3233,10 +3230,10 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
+        <v>97</v>
+      </c>
+      <c r="C30" t="s">
         <v>98</v>
-      </c>
-      <c r="C30" t="s">
-        <v>99</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>23</v>
@@ -3257,7 +3254,7 @@
         <v>24</v>
       </c>
       <c r="J30" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K30" s="13">
         <v>-12.11317</v>
@@ -3298,10 +3295,10 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
+        <v>99</v>
+      </c>
+      <c r="C31" t="s">
         <v>100</v>
-      </c>
-      <c r="C31" t="s">
-        <v>101</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>23</v>
@@ -3322,7 +3319,7 @@
         <v>24</v>
       </c>
       <c r="J31" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K31" s="13">
         <v>-12.096705</v>
@@ -3346,7 +3343,7 @@
         <v>25</v>
       </c>
       <c r="R31" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="S31" t="s">
         <v>28</v>
@@ -3363,10 +3360,10 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
+        <v>102</v>
+      </c>
+      <c r="C32" t="s">
         <v>103</v>
-      </c>
-      <c r="C32" t="s">
-        <v>104</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>23</v>
@@ -3387,7 +3384,7 @@
         <v>24</v>
       </c>
       <c r="J32" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K32" s="13">
         <v>-12.072194</v>
@@ -3428,10 +3425,10 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
+        <v>105</v>
+      </c>
+      <c r="C33" t="s">
         <v>106</v>
-      </c>
-      <c r="C33" t="s">
-        <v>107</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>23</v>
@@ -3452,7 +3449,7 @@
         <v>24</v>
       </c>
       <c r="J33" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K33" s="13">
         <v>-12.086320000000001</v>
@@ -3493,10 +3490,10 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
+        <v>107</v>
+      </c>
+      <c r="C34" t="s">
         <v>108</v>
-      </c>
-      <c r="C34" t="s">
-        <v>109</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>23</v>
@@ -3517,7 +3514,7 @@
         <v>24</v>
       </c>
       <c r="J34" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K34" s="13">
         <v>-12.02689</v>
@@ -3541,7 +3538,7 @@
         <v>29</v>
       </c>
       <c r="R34" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="S34" t="s">
         <v>28</v>
@@ -3558,10 +3555,10 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
+        <v>110</v>
+      </c>
+      <c r="C35" t="s">
         <v>111</v>
-      </c>
-      <c r="C35" t="s">
-        <v>112</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>23</v>
@@ -3582,7 +3579,7 @@
         <v>24</v>
       </c>
       <c r="J35" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K35" s="13">
         <v>-12.116166</v>
@@ -3623,10 +3620,10 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
+        <v>112</v>
+      </c>
+      <c r="C36" t="s">
         <v>113</v>
-      </c>
-      <c r="C36" t="s">
-        <v>114</v>
       </c>
       <c r="D36" s="4" t="s">
         <v>23</v>
@@ -3647,7 +3644,7 @@
         <v>24</v>
       </c>
       <c r="J36" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K36" s="13">
         <v>-12.086520999999999</v>
@@ -3688,10 +3685,10 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
+        <v>114</v>
+      </c>
+      <c r="C37" t="s">
         <v>115</v>
-      </c>
-      <c r="C37" t="s">
-        <v>116</v>
       </c>
       <c r="D37" s="4" t="s">
         <v>23</v>
@@ -3712,7 +3709,7 @@
         <v>24</v>
       </c>
       <c r="J37" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K37" s="13">
         <v>-12.13932</v>
@@ -3753,10 +3750,10 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
+        <v>116</v>
+      </c>
+      <c r="C38" t="s">
         <v>117</v>
-      </c>
-      <c r="C38" t="s">
-        <v>118</v>
       </c>
       <c r="D38" s="4" t="s">
         <v>23</v>
@@ -3777,7 +3774,7 @@
         <v>24</v>
       </c>
       <c r="J38" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K38" s="13">
         <v>-12.100669999999999</v>
@@ -3818,10 +3815,10 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
+        <v>112</v>
+      </c>
+      <c r="C39" t="s">
         <v>113</v>
-      </c>
-      <c r="C39" t="s">
-        <v>114</v>
       </c>
       <c r="D39" s="4" t="s">
         <v>23</v>
@@ -3842,7 +3839,7 @@
         <v>24</v>
       </c>
       <c r="J39" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K39" s="13">
         <v>-12.086520999999999</v>
@@ -3883,10 +3880,10 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
+        <v>118</v>
+      </c>
+      <c r="C40" t="s">
         <v>119</v>
-      </c>
-      <c r="C40" t="s">
-        <v>120</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>23</v>
@@ -3948,10 +3945,10 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
+        <v>120</v>
+      </c>
+      <c r="C41" t="s">
         <v>121</v>
-      </c>
-      <c r="C41" t="s">
-        <v>122</v>
       </c>
       <c r="D41" s="4" t="s">
         <v>23</v>
@@ -3972,7 +3969,7 @@
         <v>24</v>
       </c>
       <c r="J41" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K41" s="13">
         <v>-12.11224</v>
@@ -4013,10 +4010,10 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
+        <v>123</v>
+      </c>
+      <c r="C42" t="s">
         <v>124</v>
-      </c>
-      <c r="C42" t="s">
-        <v>125</v>
       </c>
       <c r="D42" s="4" t="s">
         <v>23</v>
@@ -4037,7 +4034,7 @@
         <v>24</v>
       </c>
       <c r="J42" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K42" s="13">
         <v>-11.97612</v>
@@ -4078,10 +4075,10 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
+        <v>69</v>
+      </c>
+      <c r="C43" t="s">
         <v>70</v>
-      </c>
-      <c r="C43" t="s">
-        <v>71</v>
       </c>
       <c r="D43" s="4" t="s">
         <v>23</v>
@@ -4102,7 +4099,7 @@
         <v>24</v>
       </c>
       <c r="J43" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K43" s="13">
         <v>-12.131688</v>
@@ -4143,10 +4140,10 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C44" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D44" s="4" t="s">
         <v>23</v>
@@ -4167,7 +4164,7 @@
         <v>24</v>
       </c>
       <c r="J44" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K44" s="13">
         <v>-12.090145</v>
@@ -4208,10 +4205,10 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
+        <v>126</v>
+      </c>
+      <c r="C45" t="s">
         <v>127</v>
-      </c>
-      <c r="C45" t="s">
-        <v>128</v>
       </c>
       <c r="D45" s="4" t="s">
         <v>23</v>
@@ -4273,10 +4270,10 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
+        <v>128</v>
+      </c>
+      <c r="C46" t="s">
         <v>129</v>
-      </c>
-      <c r="C46" t="s">
-        <v>130</v>
       </c>
       <c r="D46" s="4" t="s">
         <v>23</v>
@@ -4297,7 +4294,7 @@
         <v>24</v>
       </c>
       <c r="J46" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K46" s="13">
         <v>-12.068598</v>
@@ -4338,10 +4335,10 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
+        <v>130</v>
+      </c>
+      <c r="C47" t="s">
         <v>131</v>
-      </c>
-      <c r="C47" t="s">
-        <v>132</v>
       </c>
       <c r="D47" s="4" t="s">
         <v>23</v>
@@ -4362,7 +4359,7 @@
         <v>24</v>
       </c>
       <c r="J47" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K47" s="13">
         <v>-12.159722</v>
@@ -4403,10 +4400,10 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
+        <v>132</v>
+      </c>
+      <c r="C48" t="s">
         <v>133</v>
-      </c>
-      <c r="C48" t="s">
-        <v>134</v>
       </c>
       <c r="D48" s="4" t="s">
         <v>23</v>
@@ -4468,10 +4465,10 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
+        <v>134</v>
+      </c>
+      <c r="C49" t="s">
         <v>135</v>
-      </c>
-      <c r="C49" t="s">
-        <v>136</v>
       </c>
       <c r="D49" s="4" t="s">
         <v>23</v>
@@ -4492,7 +4489,7 @@
         <v>24</v>
       </c>
       <c r="J49" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K49" s="13">
         <v>-12.115117</v>
@@ -4533,10 +4530,10 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
+        <v>136</v>
+      </c>
+      <c r="C50" t="s">
         <v>137</v>
-      </c>
-      <c r="C50" t="s">
-        <v>138</v>
       </c>
       <c r="D50" s="4" t="s">
         <v>23</v>
@@ -4557,7 +4554,7 @@
         <v>24</v>
       </c>
       <c r="J50" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K50" s="13">
         <v>-11.9785</v>
@@ -4581,7 +4578,7 @@
         <v>32</v>
       </c>
       <c r="R50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="S50" t="s">
         <v>28</v>
@@ -4598,10 +4595,10 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
+        <v>110</v>
+      </c>
+      <c r="C51" t="s">
         <v>111</v>
-      </c>
-      <c r="C51" t="s">
-        <v>112</v>
       </c>
       <c r="D51" s="4" t="s">
         <v>23</v>
@@ -4622,7 +4619,7 @@
         <v>24</v>
       </c>
       <c r="J51" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K51" s="13">
         <v>-12.116166</v>
@@ -4663,10 +4660,10 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
+        <v>138</v>
+      </c>
+      <c r="C52" t="s">
         <v>139</v>
-      </c>
-      <c r="C52" t="s">
-        <v>140</v>
       </c>
       <c r="D52" s="4" t="s">
         <v>23</v>
@@ -4687,7 +4684,7 @@
         <v>24</v>
       </c>
       <c r="J52" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K52" s="13">
         <v>-11.989026000000001</v>
@@ -4728,10 +4725,10 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
+        <v>140</v>
+      </c>
+      <c r="C53" t="s">
         <v>141</v>
-      </c>
-      <c r="C53" t="s">
-        <v>142</v>
       </c>
       <c r="D53" s="4" t="s">
         <v>23</v>
@@ -4752,7 +4749,7 @@
         <v>24</v>
       </c>
       <c r="J53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K53" s="13">
         <v>-12.136279999999999</v>
@@ -4793,10 +4790,10 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
+        <v>142</v>
+      </c>
+      <c r="C54" t="s">
         <v>143</v>
-      </c>
-      <c r="C54" t="s">
-        <v>144</v>
       </c>
       <c r="D54" s="4" t="s">
         <v>23</v>
@@ -4858,10 +4855,10 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
+        <v>144</v>
+      </c>
+      <c r="C55" t="s">
         <v>145</v>
-      </c>
-      <c r="C55" t="s">
-        <v>146</v>
       </c>
       <c r="D55" s="4" t="s">
         <v>23</v>
@@ -4882,7 +4879,7 @@
         <v>24</v>
       </c>
       <c r="J55" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K55" s="13">
         <v>-11.9758589</v>
@@ -4897,7 +4894,7 @@
         <v>65</v>
       </c>
       <c r="O55" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P55" s="13">
         <v>-95.0918518518518</v>
@@ -4923,10 +4920,10 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
+        <v>148</v>
+      </c>
+      <c r="C56" t="s">
         <v>149</v>
-      </c>
-      <c r="C56" t="s">
-        <v>150</v>
       </c>
       <c r="D56" s="4" t="s">
         <v>23</v>
@@ -4947,7 +4944,7 @@
         <v>24</v>
       </c>
       <c r="J56" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K56" s="13">
         <v>-12.042166</v>
@@ -4962,7 +4959,7 @@
         <v>65</v>
       </c>
       <c r="O56" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P56" s="13">
         <v>-99.22</v>
@@ -4988,10 +4985,10 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
+        <v>151</v>
+      </c>
+      <c r="C57" t="s">
         <v>152</v>
-      </c>
-      <c r="C57" t="s">
-        <v>153</v>
       </c>
       <c r="D57" s="4" t="s">
         <v>23</v>
@@ -5012,7 +5009,7 @@
         <v>24</v>
       </c>
       <c r="J57" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K57" s="13">
         <v>-12.18075</v>
@@ -5027,7 +5024,7 @@
         <v>65</v>
       </c>
       <c r="O57" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P57" s="13">
         <v>-87.394074074073998</v>
@@ -5053,10 +5050,10 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
+        <v>154</v>
+      </c>
+      <c r="C58" t="s">
         <v>155</v>
-      </c>
-      <c r="C58" t="s">
-        <v>156</v>
       </c>
       <c r="D58" s="4" t="s">
         <v>23</v>
@@ -5077,7 +5074,7 @@
         <v>24</v>
       </c>
       <c r="J58" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K58" s="13">
         <v>-12.03889</v>
@@ -5092,7 +5089,7 @@
         <v>65</v>
       </c>
       <c r="O58" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P58" s="13">
         <v>-97.662222222222198</v>
@@ -5118,10 +5115,10 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
+        <v>156</v>
+      </c>
+      <c r="C59" t="s">
         <v>157</v>
-      </c>
-      <c r="C59" t="s">
-        <v>158</v>
       </c>
       <c r="D59" s="4" t="s">
         <v>23</v>
@@ -5139,10 +5136,10 @@
         <v>24</v>
       </c>
       <c r="I59" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J59" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K59" s="13">
         <v>-11.104955</v>
@@ -5157,7 +5154,7 @@
         <v>65</v>
       </c>
       <c r="O59" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P59" s="13">
         <v>-98.665925925925904</v>
@@ -5183,10 +5180,10 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
+        <v>159</v>
+      </c>
+      <c r="C60" t="s">
         <v>160</v>
-      </c>
-      <c r="C60" t="s">
-        <v>161</v>
       </c>
       <c r="D60" s="4" t="s">
         <v>23</v>
@@ -5207,7 +5204,7 @@
         <v>24</v>
       </c>
       <c r="J60" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K60" s="13">
         <v>-12.030078</v>
@@ -5222,7 +5219,7 @@
         <v>65</v>
       </c>
       <c r="O60" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P60" s="13">
         <v>-103.829629629629</v>
@@ -5248,10 +5245,10 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
+        <v>161</v>
+      </c>
+      <c r="C61" t="s">
         <v>162</v>
-      </c>
-      <c r="C61" t="s">
-        <v>163</v>
       </c>
       <c r="D61" s="4" t="s">
         <v>23</v>
@@ -5272,7 +5269,7 @@
         <v>24</v>
       </c>
       <c r="J61" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K61" s="13">
         <v>-12.029586</v>
@@ -5287,7 +5284,7 @@
         <v>65</v>
       </c>
       <c r="O61" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P61" s="13">
         <v>-105.962222222222</v>
@@ -5313,10 +5310,10 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
+        <v>163</v>
+      </c>
+      <c r="C62" t="s">
         <v>164</v>
-      </c>
-      <c r="C62" t="s">
-        <v>165</v>
       </c>
       <c r="D62" s="4" t="s">
         <v>23</v>
@@ -5337,7 +5334,7 @@
         <v>24</v>
       </c>
       <c r="J62" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="K62" s="13">
         <v>-12.054034</v>
@@ -5352,7 +5349,7 @@
         <v>65</v>
       </c>
       <c r="O62" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P62" s="13">
         <v>-105.35629629629599</v>
@@ -5378,10 +5375,10 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
+        <v>166</v>
+      </c>
+      <c r="C63" t="s">
         <v>167</v>
-      </c>
-      <c r="C63" t="s">
-        <v>168</v>
       </c>
       <c r="D63" s="4" t="s">
         <v>23</v>
@@ -5402,7 +5399,7 @@
         <v>24</v>
       </c>
       <c r="J63" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="K63" s="13">
         <v>-12.220281</v>
@@ -5417,7 +5414,7 @@
         <v>65</v>
       </c>
       <c r="O63" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P63" s="13">
         <v>-106.46592592592501</v>
@@ -5443,10 +5440,10 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
+        <v>169</v>
+      </c>
+      <c r="C64" t="s">
         <v>170</v>
-      </c>
-      <c r="C64" t="s">
-        <v>171</v>
       </c>
       <c r="D64" s="4" t="s">
         <v>23</v>
@@ -5467,7 +5464,7 @@
         <v>24</v>
       </c>
       <c r="J64" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="K64" s="13">
         <v>-11.920861</v>
@@ -5482,7 +5479,7 @@
         <v>65</v>
       </c>
       <c r="O64" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P64" s="13">
         <v>-106.99481481481401</v>
@@ -5508,10 +5505,10 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
+        <v>172</v>
+      </c>
+      <c r="C65" t="s">
         <v>173</v>
-      </c>
-      <c r="C65" t="s">
-        <v>174</v>
       </c>
       <c r="D65" s="4" t="s">
         <v>23</v>
@@ -5532,7 +5529,7 @@
         <v>24</v>
       </c>
       <c r="J65" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="K65" s="13">
         <v>-12.030010000000001</v>
@@ -5547,7 +5544,7 @@
         <v>65</v>
       </c>
       <c r="O65" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P65" s="13">
         <v>-105.65037037037</v>
@@ -5573,10 +5570,10 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
+        <v>175</v>
+      </c>
+      <c r="C66" t="s">
         <v>176</v>
-      </c>
-      <c r="C66" t="s">
-        <v>177</v>
       </c>
       <c r="D66" s="4" t="s">
         <v>23</v>
@@ -5594,10 +5591,10 @@
         <v>24</v>
       </c>
       <c r="I66" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J66" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K66" s="13">
         <v>-11.96794</v>
@@ -5612,7 +5609,7 @@
         <v>65</v>
       </c>
       <c r="O66" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P66" s="13">
         <v>-106.094074074074</v>
@@ -5638,10 +5635,10 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
+        <v>177</v>
+      </c>
+      <c r="C67" t="s">
         <v>178</v>
-      </c>
-      <c r="C67" t="s">
-        <v>179</v>
       </c>
       <c r="D67" s="4" t="s">
         <v>23</v>
@@ -5659,10 +5656,10 @@
         <v>24</v>
       </c>
       <c r="I67" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J67" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K67" s="13">
         <v>-11.983639999999999</v>
@@ -5677,7 +5674,7 @@
         <v>65</v>
       </c>
       <c r="O67" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P67" s="13">
         <v>-101.63407407407399</v>
@@ -5703,10 +5700,10 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
+        <v>179</v>
+      </c>
+      <c r="C68" t="s">
         <v>180</v>
-      </c>
-      <c r="C68" t="s">
-        <v>181</v>
       </c>
       <c r="D68" s="4" t="s">
         <v>23</v>
@@ -5724,10 +5721,10 @@
         <v>24</v>
       </c>
       <c r="I68" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J68" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K68" s="13">
         <v>-11.97894</v>
@@ -5742,7 +5739,7 @@
         <v>65</v>
       </c>
       <c r="O68" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P68" s="13">
         <v>-101.81037037036999</v>
@@ -5768,10 +5765,10 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
+        <v>181</v>
+      </c>
+      <c r="C69" t="s">
         <v>182</v>
-      </c>
-      <c r="C69" t="s">
-        <v>183</v>
       </c>
       <c r="D69" s="4" t="s">
         <v>23</v>
@@ -5792,7 +5789,7 @@
         <v>24</v>
       </c>
       <c r="J69" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K69" s="13">
         <v>-11.999530999999999</v>
@@ -5807,7 +5804,7 @@
         <v>65</v>
       </c>
       <c r="O69" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P69" s="13">
         <v>-105.034814814814</v>
@@ -5833,10 +5830,10 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
+        <v>183</v>
+      </c>
+      <c r="C70" t="s">
         <v>184</v>
-      </c>
-      <c r="C70" t="s">
-        <v>185</v>
       </c>
       <c r="D70" s="4" t="s">
         <v>23</v>
@@ -5857,7 +5854,7 @@
         <v>24</v>
       </c>
       <c r="J70" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K70" s="13">
         <v>-11.968056000000001</v>
@@ -5872,7 +5869,7 @@
         <v>65</v>
       </c>
       <c r="O70" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P70" s="13">
         <v>-105.888888888888</v>
@@ -5898,10 +5895,10 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
+        <v>185</v>
+      </c>
+      <c r="C71" t="s">
         <v>186</v>
-      </c>
-      <c r="C71" t="s">
-        <v>187</v>
       </c>
       <c r="D71" s="4" t="s">
         <v>23</v>
@@ -5922,7 +5919,7 @@
         <v>24</v>
       </c>
       <c r="J71" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K71" s="13">
         <v>-12.013356999999999</v>
@@ -5937,7 +5934,7 @@
         <v>65</v>
       </c>
       <c r="O71" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P71" s="13">
         <v>-106.408148148148</v>
@@ -5963,10 +5960,10 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
+        <v>187</v>
+      </c>
+      <c r="C72" t="s">
         <v>188</v>
-      </c>
-      <c r="C72" t="s">
-        <v>189</v>
       </c>
       <c r="D72" s="4" t="s">
         <v>23</v>
@@ -5987,7 +5984,7 @@
         <v>24</v>
       </c>
       <c r="J72" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="K72" s="13">
         <v>-11.99104</v>
@@ -6002,7 +5999,7 @@
         <v>65</v>
       </c>
       <c r="O72" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P72" s="13">
         <v>-107.534074074074</v>
@@ -6011,7 +6008,7 @@
         <v>37</v>
       </c>
       <c r="R72" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="S72" t="s">
         <v>28</v>
@@ -6028,10 +6025,10 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
+        <v>189</v>
+      </c>
+      <c r="C73" t="s">
         <v>190</v>
-      </c>
-      <c r="C73" t="s">
-        <v>191</v>
       </c>
       <c r="D73" s="4" t="s">
         <v>23</v>
@@ -6052,7 +6049,7 @@
         <v>24</v>
       </c>
       <c r="J73" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="K73" s="13">
         <v>-11.915039999999999</v>
@@ -6067,7 +6064,7 @@
         <v>65</v>
       </c>
       <c r="O73" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P73" s="13">
         <v>-104.68074074074001</v>
@@ -6093,10 +6090,10 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
+        <v>191</v>
+      </c>
+      <c r="C74" t="s">
         <v>192</v>
-      </c>
-      <c r="C74" t="s">
-        <v>193</v>
       </c>
       <c r="D74" s="4" t="s">
         <v>23</v>
@@ -6117,7 +6114,7 @@
         <v>24</v>
       </c>
       <c r="J74" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="K74" s="13">
         <v>-11.96102</v>
@@ -6132,7 +6129,7 @@
         <v>65</v>
       </c>
       <c r="O74" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P74" s="13">
         <v>-106.73960784313699</v>
@@ -6158,10 +6155,10 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
+        <v>193</v>
+      </c>
+      <c r="C75" t="s">
         <v>194</v>
-      </c>
-      <c r="C75" t="s">
-        <v>195</v>
       </c>
       <c r="D75" s="4" t="s">
         <v>23</v>
@@ -6182,7 +6179,7 @@
         <v>24</v>
       </c>
       <c r="J75" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="K75" s="13">
         <v>-12.025022</v>
@@ -6197,7 +6194,7 @@
         <v>65</v>
       </c>
       <c r="O75" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P75" s="13">
         <v>-106.427407407407</v>
@@ -6223,10 +6220,10 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
+        <v>195</v>
+      </c>
+      <c r="C76" t="s">
         <v>196</v>
-      </c>
-      <c r="C76" t="s">
-        <v>197</v>
       </c>
       <c r="D76" s="4" t="s">
         <v>23</v>
@@ -6247,7 +6244,7 @@
         <v>24</v>
       </c>
       <c r="J76" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K76" s="13">
         <v>-12.024207000000001</v>
@@ -6262,7 +6259,7 @@
         <v>65</v>
       </c>
       <c r="O76" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P76" s="13">
         <v>-103.314074074074</v>
@@ -6288,10 +6285,10 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
+        <v>197</v>
+      </c>
+      <c r="C77" t="s">
         <v>198</v>
-      </c>
-      <c r="C77" t="s">
-        <v>199</v>
       </c>
       <c r="D77" s="4" t="s">
         <v>23</v>
@@ -6312,7 +6309,7 @@
         <v>24</v>
       </c>
       <c r="J77" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="K77" s="13">
         <v>-11.86243</v>
@@ -6327,7 +6324,7 @@
         <v>65</v>
       </c>
       <c r="O77" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P77" s="13">
         <v>-104.246666666666</v>
@@ -6353,10 +6350,10 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
+        <v>200</v>
+      </c>
+      <c r="C78" t="s">
         <v>201</v>
-      </c>
-      <c r="C78" t="s">
-        <v>202</v>
       </c>
       <c r="D78" s="4" t="s">
         <v>23</v>
@@ -6377,7 +6374,7 @@
         <v>24</v>
       </c>
       <c r="J78" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="K78" s="13">
         <v>-12.013028</v>
@@ -6392,7 +6389,7 @@
         <v>65</v>
       </c>
       <c r="O78" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P78" s="13">
         <v>-105.59555555555499</v>
@@ -6418,10 +6415,10 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
+        <v>202</v>
+      </c>
+      <c r="C79" t="s">
         <v>203</v>
-      </c>
-      <c r="C79" t="s">
-        <v>204</v>
       </c>
       <c r="D79" s="4" t="s">
         <v>23</v>
@@ -6442,7 +6439,7 @@
         <v>24</v>
       </c>
       <c r="J79" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="K79" s="13">
         <v>-12.038003</v>
@@ -6457,7 +6454,7 @@
         <v>65</v>
       </c>
       <c r="O79" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P79" s="13">
         <v>-107.753333333333</v>
@@ -6483,10 +6480,10 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
+        <v>205</v>
+      </c>
+      <c r="C80" t="s">
         <v>206</v>
-      </c>
-      <c r="C80" t="s">
-        <v>207</v>
       </c>
       <c r="D80" s="4" t="s">
         <v>23</v>
@@ -6507,7 +6504,7 @@
         <v>24</v>
       </c>
       <c r="J80" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K80" s="13">
         <v>-12.02073</v>
@@ -6522,7 +6519,7 @@
         <v>65</v>
       </c>
       <c r="O80" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P80" s="13">
         <v>-106.46592592592501</v>
@@ -6548,10 +6545,10 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
+        <v>207</v>
+      </c>
+      <c r="C81" t="s">
         <v>208</v>
-      </c>
-      <c r="C81" t="s">
-        <v>209</v>
       </c>
       <c r="D81" s="4" t="s">
         <v>23</v>
@@ -6572,7 +6569,7 @@
         <v>24</v>
       </c>
       <c r="J81" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="K81" s="13">
         <v>-12.198600000000001</v>
@@ -6587,7 +6584,7 @@
         <v>65</v>
       </c>
       <c r="O81" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P81" s="13">
         <v>-104.21407407407401</v>
@@ -6613,10 +6610,10 @@
         <v>81</v>
       </c>
       <c r="B82" t="s">
+        <v>197</v>
+      </c>
+      <c r="C82" t="s">
         <v>198</v>
-      </c>
-      <c r="C82" t="s">
-        <v>199</v>
       </c>
       <c r="D82" s="4" t="s">
         <v>23</v>
@@ -6637,7 +6634,7 @@
         <v>24</v>
       </c>
       <c r="J82" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="K82" s="13">
         <v>-11.86243</v>
@@ -6652,7 +6649,7 @@
         <v>65</v>
       </c>
       <c r="O82" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P82" s="13">
         <v>-103.583529411764</v>
@@ -6678,10 +6675,10 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
+        <v>209</v>
+      </c>
+      <c r="C83" t="s">
         <v>210</v>
-      </c>
-      <c r="C83" t="s">
-        <v>211</v>
       </c>
       <c r="D83" s="4" t="s">
         <v>23</v>
@@ -6702,7 +6699,7 @@
         <v>24</v>
       </c>
       <c r="J83" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="K83" s="13">
         <v>-12.057002000000001</v>
@@ -6717,7 +6714,7 @@
         <v>65</v>
       </c>
       <c r="O83" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P83" s="13">
         <v>-104.645925925925</v>
@@ -6743,10 +6740,10 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
+        <v>191</v>
+      </c>
+      <c r="C84" t="s">
         <v>192</v>
-      </c>
-      <c r="C84" t="s">
-        <v>193</v>
       </c>
       <c r="D84" s="4" t="s">
         <v>23</v>
@@ -6767,7 +6764,7 @@
         <v>24</v>
       </c>
       <c r="J84" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="K84" s="13">
         <v>-11.96102</v>
@@ -6782,7 +6779,7 @@
         <v>65</v>
       </c>
       <c r="O84" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P84" s="13">
         <v>-107.118431372549</v>
@@ -6808,10 +6805,10 @@
         <v>84</v>
       </c>
       <c r="B85" t="s">
+        <v>183</v>
+      </c>
+      <c r="C85" t="s">
         <v>184</v>
-      </c>
-      <c r="C85" t="s">
-        <v>185</v>
       </c>
       <c r="D85" s="4" t="s">
         <v>23</v>
@@ -6832,7 +6829,7 @@
         <v>24</v>
       </c>
       <c r="J85" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K85" s="13">
         <v>-11.968056000000001</v>
@@ -6847,7 +6844,7 @@
         <v>65</v>
       </c>
       <c r="O85" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P85" s="13">
         <v>-103.49629629629599</v>
@@ -6873,10 +6870,10 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
+        <v>211</v>
+      </c>
+      <c r="C86" t="s">
         <v>212</v>
-      </c>
-      <c r="C86" t="s">
-        <v>213</v>
       </c>
       <c r="D86" s="4" t="s">
         <v>23</v>
@@ -6897,7 +6894,7 @@
         <v>24</v>
       </c>
       <c r="J86" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K86" s="13">
         <v>-11.953249</v>
@@ -6912,7 +6909,7 @@
         <v>65</v>
       </c>
       <c r="O86" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P86" s="13">
         <v>-105.47703703703699</v>
@@ -6938,10 +6935,10 @@
         <v>86</v>
       </c>
       <c r="B87" t="s">
+        <v>213</v>
+      </c>
+      <c r="C87" t="s">
         <v>214</v>
-      </c>
-      <c r="C87" t="s">
-        <v>215</v>
       </c>
       <c r="D87" s="4" t="s">
         <v>23</v>
@@ -6962,7 +6959,7 @@
         <v>24</v>
       </c>
       <c r="J87" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="K87" s="13">
         <v>-11.956327</v>
@@ -6977,7 +6974,7 @@
         <v>65</v>
       </c>
       <c r="O87" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P87" s="13">
         <v>-107.794814814814</v>
@@ -6986,7 +6983,7 @@
         <v>36</v>
       </c>
       <c r="R87" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="S87" t="s">
         <v>28</v>
@@ -7003,10 +7000,10 @@
         <v>87</v>
       </c>
       <c r="B88" t="s">
+        <v>215</v>
+      </c>
+      <c r="C88" t="s">
         <v>216</v>
-      </c>
-      <c r="C88" t="s">
-        <v>217</v>
       </c>
       <c r="D88" s="4" t="s">
         <v>23</v>
@@ -7027,7 +7024,7 @@
         <v>24</v>
       </c>
       <c r="J88" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="K88" s="13">
         <v>-12.161808000000001</v>
@@ -7042,7 +7039,7 @@
         <v>65</v>
       </c>
       <c r="O88" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P88" s="13">
         <v>-107.814814814814</v>
@@ -7051,7 +7048,7 @@
         <v>26</v>
       </c>
       <c r="R88" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="S88" t="s">
         <v>28</v>
@@ -7068,10 +7065,10 @@
         <v>88</v>
       </c>
       <c r="B89" t="s">
+        <v>218</v>
+      </c>
+      <c r="C89" t="s">
         <v>219</v>
-      </c>
-      <c r="C89" t="s">
-        <v>220</v>
       </c>
       <c r="D89" s="4" t="s">
         <v>23</v>
@@ -7092,7 +7089,7 @@
         <v>24</v>
       </c>
       <c r="J89" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="K89" s="13">
         <v>-12.19285</v>
@@ -7107,7 +7104,7 @@
         <v>65</v>
       </c>
       <c r="O89" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P89" s="13">
         <v>-104.01629629629601</v>
@@ -7133,10 +7130,10 @@
         <v>89</v>
       </c>
       <c r="B90" t="s">
+        <v>220</v>
+      </c>
+      <c r="C90" t="s">
         <v>221</v>
-      </c>
-      <c r="C90" t="s">
-        <v>222</v>
       </c>
       <c r="D90" s="4" t="s">
         <v>23</v>
@@ -7157,7 +7154,7 @@
         <v>24</v>
       </c>
       <c r="J90" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="K90" s="13">
         <v>-12.0529744</v>
@@ -7172,7 +7169,7 @@
         <v>65</v>
       </c>
       <c r="O90" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P90" s="13">
         <v>-106.02592592592499</v>
@@ -7198,10 +7195,10 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
+        <v>222</v>
+      </c>
+      <c r="C91" t="s">
         <v>223</v>
-      </c>
-      <c r="C91" t="s">
-        <v>224</v>
       </c>
       <c r="D91" s="4" t="s">
         <v>23</v>
@@ -7222,7 +7219,7 @@
         <v>24</v>
       </c>
       <c r="J91" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="K91" s="13">
         <v>-11.871293</v>
@@ -7237,7 +7234,7 @@
         <v>65</v>
       </c>
       <c r="O91" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P91" s="13">
         <v>-108.074814814814</v>
@@ -7246,7 +7243,7 @@
         <v>21</v>
       </c>
       <c r="R91" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="S91" t="s">
         <v>28</v>
@@ -7263,10 +7260,10 @@
         <v>91</v>
       </c>
       <c r="B92" t="s">
+        <v>225</v>
+      </c>
+      <c r="C92" t="s">
         <v>226</v>
-      </c>
-      <c r="C92" t="s">
-        <v>227</v>
       </c>
       <c r="D92" s="4" t="s">
         <v>23</v>
@@ -7287,7 +7284,7 @@
         <v>24</v>
       </c>
       <c r="J92" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K92" s="13">
         <v>-12.02774</v>
@@ -7302,7 +7299,7 @@
         <v>65</v>
       </c>
       <c r="O92" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P92" s="13">
         <v>-102.524444444444</v>
@@ -7328,10 +7325,10 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
+        <v>227</v>
+      </c>
+      <c r="C93" t="s">
         <v>228</v>
-      </c>
-      <c r="C93" t="s">
-        <v>229</v>
       </c>
       <c r="D93" s="4" t="s">
         <v>23</v>
@@ -7352,7 +7349,7 @@
         <v>24</v>
       </c>
       <c r="J93" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K93" s="13">
         <v>-12.06522</v>
@@ -7367,7 +7364,7 @@
         <v>65</v>
       </c>
       <c r="O93" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P93" s="13">
         <v>-104.34444444444399</v>
@@ -7393,10 +7390,10 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
+        <v>229</v>
+      </c>
+      <c r="C94" t="s">
         <v>230</v>
-      </c>
-      <c r="C94" t="s">
-        <v>231</v>
       </c>
       <c r="D94" s="4" t="s">
         <v>23</v>
@@ -7414,10 +7411,10 @@
         <v>24</v>
       </c>
       <c r="I94" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J94" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K94" s="13">
         <v>-12.042149999999999</v>
@@ -7432,7 +7429,7 @@
         <v>65</v>
       </c>
       <c r="O94" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P94" s="13">
         <v>-104.282962962962</v>
@@ -7458,10 +7455,10 @@
         <v>94</v>
       </c>
       <c r="B95" t="s">
+        <v>231</v>
+      </c>
+      <c r="C95" t="s">
         <v>232</v>
-      </c>
-      <c r="C95" t="s">
-        <v>233</v>
       </c>
       <c r="D95" s="4" t="s">
         <v>23</v>
@@ -7482,7 +7479,7 @@
         <v>24</v>
       </c>
       <c r="J95" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="K95" s="13">
         <v>-12.216100000000001</v>
@@ -7497,7 +7494,7 @@
         <v>65</v>
       </c>
       <c r="O95" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P95" s="13">
         <v>-104.529629629629</v>
@@ -7523,10 +7520,10 @@
         <v>95</v>
       </c>
       <c r="B96" t="s">
+        <v>193</v>
+      </c>
+      <c r="C96" t="s">
         <v>194</v>
-      </c>
-      <c r="C96" t="s">
-        <v>195</v>
       </c>
       <c r="D96" s="4" t="s">
         <v>23</v>
@@ -7547,7 +7544,7 @@
         <v>24</v>
       </c>
       <c r="J96" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="K96" s="13">
         <v>-12.025022</v>
@@ -7562,7 +7559,7 @@
         <v>65</v>
       </c>
       <c r="O96" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P96" s="13">
         <v>-106.89555555555501</v>
@@ -7588,10 +7585,10 @@
         <v>96</v>
       </c>
       <c r="B97" t="s">
+        <v>233</v>
+      </c>
+      <c r="C97" t="s">
         <v>234</v>
-      </c>
-      <c r="C97" t="s">
-        <v>235</v>
       </c>
       <c r="D97" s="4" t="s">
         <v>23</v>
@@ -7609,10 +7606,10 @@
         <v>24</v>
       </c>
       <c r="I97" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J97" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K97" s="13">
         <v>-12.02453</v>
@@ -7627,7 +7624,7 @@
         <v>65</v>
       </c>
       <c r="O97" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P97" s="13">
         <v>-104.636296296296</v>
@@ -7653,10 +7650,10 @@
         <v>97</v>
       </c>
       <c r="B98" t="s">
+        <v>235</v>
+      </c>
+      <c r="C98" t="s">
         <v>236</v>
-      </c>
-      <c r="C98" t="s">
-        <v>237</v>
       </c>
       <c r="D98" s="4" t="s">
         <v>23</v>
@@ -7677,7 +7674,7 @@
         <v>24</v>
       </c>
       <c r="J98" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="K98" s="13">
         <v>-11.956438199999999</v>
@@ -7692,7 +7689,7 @@
         <v>65</v>
       </c>
       <c r="O98" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P98" s="13">
         <v>-105.978518518518</v>
@@ -7718,10 +7715,10 @@
         <v>98</v>
       </c>
       <c r="B99" t="s">
+        <v>215</v>
+      </c>
+      <c r="C99" t="s">
         <v>216</v>
-      </c>
-      <c r="C99" t="s">
-        <v>217</v>
       </c>
       <c r="D99" s="4" t="s">
         <v>23</v>
@@ -7742,7 +7739,7 @@
         <v>24</v>
       </c>
       <c r="J99" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="K99" s="13">
         <v>-12.161808000000001</v>
@@ -7757,7 +7754,7 @@
         <v>65</v>
       </c>
       <c r="O99" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P99" s="13">
         <v>-102.98222222222201</v>
@@ -7783,10 +7780,10 @@
         <v>99</v>
       </c>
       <c r="B100" t="s">
+        <v>237</v>
+      </c>
+      <c r="C100" t="s">
         <v>238</v>
-      </c>
-      <c r="C100" t="s">
-        <v>239</v>
       </c>
       <c r="D100" s="4" t="s">
         <v>23</v>
@@ -7807,7 +7804,7 @@
         <v>24</v>
       </c>
       <c r="J100" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="K100" s="13">
         <v>-11.92686</v>
@@ -7822,7 +7819,7 @@
         <v>65</v>
       </c>
       <c r="O100" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P100" s="13">
         <v>-103.60074074073999</v>
@@ -7848,10 +7845,10 @@
         <v>100</v>
       </c>
       <c r="B101" t="s">
+        <v>240</v>
+      </c>
+      <c r="C101" t="s">
         <v>241</v>
-      </c>
-      <c r="C101" t="s">
-        <v>242</v>
       </c>
       <c r="D101" s="4" t="s">
         <v>23</v>
@@ -7872,7 +7869,7 @@
         <v>24</v>
       </c>
       <c r="J101" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="K101" s="13">
         <v>-11.847770000000001</v>
@@ -7887,7 +7884,7 @@
         <v>65</v>
       </c>
       <c r="O101" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P101" s="13">
         <v>-108.61037037037001</v>
@@ -7896,7 +7893,7 @@
         <v>32</v>
       </c>
       <c r="R101" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="S101" t="s">
         <v>28</v>
@@ -7913,10 +7910,10 @@
         <v>101</v>
       </c>
       <c r="B102" t="s">
+        <v>242</v>
+      </c>
+      <c r="C102" t="s">
         <v>243</v>
-      </c>
-      <c r="C102" t="s">
-        <v>244</v>
       </c>
       <c r="D102" s="4" t="s">
         <v>23</v>
@@ -7934,10 +7931,10 @@
         <v>24</v>
       </c>
       <c r="I102" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J102" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="K102" s="13">
         <v>-11.859475</v>
@@ -7952,7 +7949,7 @@
         <v>65</v>
       </c>
       <c r="O102" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="P102" s="13">
         <v>-96.910370370370302</v>
@@ -7978,10 +7975,10 @@
         <v>102</v>
       </c>
       <c r="B103" t="s">
+        <v>246</v>
+      </c>
+      <c r="C103" t="s">
         <v>247</v>
-      </c>
-      <c r="C103" t="s">
-        <v>248</v>
       </c>
       <c r="D103" s="4" t="s">
         <v>23</v>
@@ -8002,7 +7999,7 @@
         <v>24</v>
       </c>
       <c r="J103" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="K103" s="13">
         <v>-12.251481</v>
@@ -8017,7 +8014,7 @@
         <v>65</v>
       </c>
       <c r="O103" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="P103" s="13">
         <v>-102.406666666666</v>
@@ -8043,10 +8040,10 @@
         <v>103</v>
       </c>
       <c r="B104" t="s">
+        <v>249</v>
+      </c>
+      <c r="C104" t="s">
         <v>250</v>
-      </c>
-      <c r="C104" t="s">
-        <v>251</v>
       </c>
       <c r="D104" s="4" t="s">
         <v>23</v>
@@ -8064,10 +8061,10 @@
         <v>24</v>
       </c>
       <c r="I104" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J104" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="K104" s="13">
         <v>-11.881847</v>
@@ -8082,7 +8079,7 @@
         <v>65</v>
       </c>
       <c r="O104" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="P104" s="13">
         <v>-99.942962962962895</v>
@@ -8108,10 +8105,10 @@
         <v>104</v>
       </c>
       <c r="B105" t="s">
+        <v>251</v>
+      </c>
+      <c r="C105" t="s">
         <v>252</v>
-      </c>
-      <c r="C105" t="s">
-        <v>253</v>
       </c>
       <c r="D105" s="4" t="s">
         <v>23</v>
@@ -8132,7 +8129,7 @@
         <v>24</v>
       </c>
       <c r="J105" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="K105" s="13">
         <v>-11.968400000000001</v>
@@ -8147,7 +8144,7 @@
         <v>65</v>
       </c>
       <c r="O105" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="P105" s="13">
         <v>-101.785185185185</v>
@@ -8173,10 +8170,10 @@
         <v>105</v>
       </c>
       <c r="B106" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C106" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D106" s="4" t="s">
         <v>23</v>
@@ -8197,7 +8194,7 @@
         <v>24</v>
       </c>
       <c r="J106" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="K106" s="13">
         <v>-12.275888999999999</v>
@@ -8212,7 +8209,7 @@
         <v>65</v>
       </c>
       <c r="O106" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="P106" s="13">
         <v>-108.246666666666</v>
@@ -8221,7 +8218,7 @@
         <v>34</v>
       </c>
       <c r="R106" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="S106" t="s">
         <v>28</v>
@@ -8238,10 +8235,10 @@
         <v>106</v>
       </c>
       <c r="B107" t="s">
+        <v>255</v>
+      </c>
+      <c r="C107" t="s">
         <v>256</v>
-      </c>
-      <c r="C107" t="s">
-        <v>257</v>
       </c>
       <c r="D107" s="4" t="s">
         <v>23</v>
@@ -8262,7 +8259,7 @@
         <v>24</v>
       </c>
       <c r="J107" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="K107" s="13">
         <v>-11.972149999999999</v>
@@ -8277,7 +8274,7 @@
         <v>65</v>
       </c>
       <c r="O107" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="P107" s="13">
         <v>-100.271111111111</v>
@@ -8303,10 +8300,10 @@
         <v>107</v>
       </c>
       <c r="B108" t="s">
+        <v>257</v>
+      </c>
+      <c r="C108" t="s">
         <v>258</v>
-      </c>
-      <c r="C108" t="s">
-        <v>259</v>
       </c>
       <c r="D108" s="4" t="s">
         <v>23</v>
@@ -8327,7 +8324,7 @@
         <v>24</v>
       </c>
       <c r="J108" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="K108" s="13">
         <v>-12.0072741</v>
@@ -8342,7 +8339,7 @@
         <v>65</v>
       </c>
       <c r="O108" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="P108" s="13">
         <v>-105.473333333333</v>
@@ -8368,10 +8365,10 @@
         <v>108</v>
       </c>
       <c r="B109" t="s">
+        <v>259</v>
+      </c>
+      <c r="C109" t="s">
         <v>260</v>
-      </c>
-      <c r="C109" t="s">
-        <v>261</v>
       </c>
       <c r="D109" s="4" t="s">
         <v>23</v>
@@ -8392,7 +8389,7 @@
         <v>24</v>
       </c>
       <c r="J109" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="K109" s="13">
         <v>-12.390222</v>
@@ -8407,7 +8404,7 @@
         <v>65</v>
       </c>
       <c r="O109" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="P109" s="13">
         <v>-107.805925925925</v>
@@ -8433,10 +8430,10 @@
         <v>109</v>
       </c>
       <c r="B110" t="s">
+        <v>262</v>
+      </c>
+      <c r="C110" t="s">
         <v>263</v>
-      </c>
-      <c r="C110" t="s">
-        <v>264</v>
       </c>
       <c r="D110" s="4" t="s">
         <v>23</v>
@@ -8457,7 +8454,7 @@
         <v>24</v>
       </c>
       <c r="J110" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="K110" s="13">
         <v>-12.087128</v>
@@ -8472,7 +8469,7 @@
         <v>65</v>
       </c>
       <c r="O110" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="P110" s="13">
         <v>-107.425185185185</v>
@@ -8498,10 +8495,10 @@
         <v>110</v>
       </c>
       <c r="B111" t="s">
+        <v>265</v>
+      </c>
+      <c r="C111" t="s">
         <v>266</v>
-      </c>
-      <c r="C111" t="s">
-        <v>267</v>
       </c>
       <c r="D111" s="4" t="s">
         <v>23</v>
@@ -8519,10 +8516,10 @@
         <v>24</v>
       </c>
       <c r="I111" t="s">
+        <v>267</v>
+      </c>
+      <c r="J111" t="s">
         <v>268</v>
-      </c>
-      <c r="J111" t="s">
-        <v>269</v>
       </c>
       <c r="K111" s="13">
         <v>-12.983219999999999</v>
@@ -8537,7 +8534,7 @@
         <v>65</v>
       </c>
       <c r="O111" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="P111" s="13">
         <v>-93.2681481481481</v>
@@ -8563,10 +8560,10 @@
         <v>111</v>
       </c>
       <c r="B112" t="s">
+        <v>270</v>
+      </c>
+      <c r="C112" t="s">
         <v>271</v>
-      </c>
-      <c r="C112" t="s">
-        <v>272</v>
       </c>
       <c r="D112" s="4" t="s">
         <v>23</v>
@@ -8584,10 +8581,10 @@
         <v>24</v>
       </c>
       <c r="I112" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="J112" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="K112" s="13">
         <v>-12.807699</v>
@@ -8602,7 +8599,7 @@
         <v>65</v>
       </c>
       <c r="O112" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="P112" s="13">
         <v>-98.331111111110999</v>
@@ -8628,10 +8625,10 @@
         <v>112</v>
       </c>
       <c r="B113" t="s">
+        <v>273</v>
+      </c>
+      <c r="C113" t="s">
         <v>274</v>
-      </c>
-      <c r="C113" t="s">
-        <v>275</v>
       </c>
       <c r="D113" s="4" t="s">
         <v>23</v>
@@ -8649,10 +8646,10 @@
         <v>24</v>
       </c>
       <c r="I113" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="J113" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="K113" s="13">
         <v>-12.948840000000001</v>
@@ -8667,7 +8664,7 @@
         <v>65</v>
       </c>
       <c r="O113" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="P113" s="13">
         <v>-95.282222222222202</v>
@@ -8693,10 +8690,10 @@
         <v>113</v>
       </c>
       <c r="B114" t="s">
+        <v>276</v>
+      </c>
+      <c r="C114" t="s">
         <v>277</v>
-      </c>
-      <c r="C114" t="s">
-        <v>278</v>
       </c>
       <c r="D114" s="4" t="s">
         <v>23</v>
@@ -8717,7 +8714,7 @@
         <v>24</v>
       </c>
       <c r="J114" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K114" s="13">
         <v>-12.460699999999999</v>
@@ -8732,7 +8729,7 @@
         <v>65</v>
       </c>
       <c r="O114" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="P114" s="13">
         <v>-104.979259259259</v>

</xml_diff>